<commit_message>
latetimepoints added -- fix needed
</commit_message>
<xml_diff>
--- a/datafiles/NEW_CAR_fractions_TD_response.xlsx
+++ b/datafiles/NEW_CAR_fractions_TD_response.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10507"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanketrane/Dropbox/MZ_munich/Datafiles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanketrane/Desktop/Work/cmdstan/MZ_munich/datafiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04612BA9-178E-BF46-A562-E16D8EEBEAC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F9465E6-E29B-0542-B5FA-18445FCEF55D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="26420" windowHeight="21500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="40800" windowHeight="22500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="16">
   <si>
     <t>genotype</t>
   </si>
@@ -470,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N81"/>
+  <dimension ref="A1:N92"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="196" zoomScaleNormal="196" zoomScaleSheetLayoutView="50" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" zoomScale="188" zoomScaleNormal="188" zoomScaleSheetLayoutView="50" workbookViewId="0">
+      <selection sqref="A1:M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -492,7 +492,7 @@
     <col min="13" max="13" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="2" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -3453,331 +3453,782 @@
         <v>18.3</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B74" s="1">
+        <v>17</v>
+      </c>
+      <c r="C74" s="3">
+        <v>102</v>
+      </c>
+      <c r="D74" s="3">
+        <v>47</v>
+      </c>
+      <c r="E74" s="3">
+        <v>4.8899999999999997</v>
+      </c>
+      <c r="F74" s="3">
+        <v>73.599999999999994</v>
+      </c>
+      <c r="G74" s="3">
+        <v>2.35</v>
+      </c>
+      <c r="H74" s="3">
+        <v>5.95</v>
+      </c>
+      <c r="I74" s="3">
+        <v>2.7</v>
+      </c>
+      <c r="J74" s="3">
+        <v>3.56</v>
+      </c>
+      <c r="K74" s="3">
+        <v>89.6</v>
+      </c>
+      <c r="L74" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="M74" s="3">
+        <v>14.6</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B75" s="1">
+        <v>17</v>
+      </c>
+      <c r="C75" s="3">
+        <v>85</v>
+      </c>
+      <c r="D75" s="3">
+        <v>53</v>
+      </c>
+      <c r="E75" s="3">
+        <v>3.81</v>
+      </c>
+      <c r="F75" s="3">
+        <v>74.2</v>
+      </c>
+      <c r="G75" s="3">
+        <v>1.67</v>
+      </c>
+      <c r="H75" s="3">
+        <v>4.92</v>
+      </c>
+      <c r="I75" s="3">
+        <v>4.54</v>
+      </c>
+      <c r="J75" s="3">
+        <v>3.85</v>
+      </c>
+      <c r="K75" s="3">
+        <v>65.400000000000006</v>
+      </c>
+      <c r="L75" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="M75" s="3">
+        <v>17.8</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B76" s="1">
+        <v>17</v>
+      </c>
+      <c r="C76" s="3">
+        <v>83.7</v>
+      </c>
+      <c r="D76" s="3">
+        <v>54.1</v>
+      </c>
+      <c r="E76" s="3">
+        <v>4.12</v>
+      </c>
+      <c r="F76" s="3">
+        <v>71.8</v>
+      </c>
+      <c r="G76" s="3">
+        <v>3.05</v>
+      </c>
+      <c r="H76" s="3">
+        <v>5.28</v>
+      </c>
+      <c r="I76" s="3">
+        <v>4.49</v>
+      </c>
+      <c r="J76" s="3">
+        <v>2.98</v>
+      </c>
+      <c r="K76" s="3">
+        <v>70.3</v>
+      </c>
+      <c r="L76" s="3">
+        <v>0.42</v>
+      </c>
+      <c r="M76" s="3">
+        <v>13.1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B77" s="1">
+        <v>22</v>
+      </c>
+      <c r="C77" s="3">
+        <v>75</v>
+      </c>
+      <c r="D77" s="3">
+        <v>53.3</v>
+      </c>
+      <c r="E77" s="3">
+        <v>2.82</v>
+      </c>
+      <c r="F77" s="3">
+        <v>73.599999999999994</v>
+      </c>
+      <c r="G77" s="3">
+        <v>1.66</v>
+      </c>
+      <c r="H77" s="3">
+        <v>4.55</v>
+      </c>
+      <c r="I77" s="3">
+        <v>2.25</v>
+      </c>
+      <c r="J77" s="3">
+        <v>1.88</v>
+      </c>
+      <c r="K77" s="3">
+        <v>75.599999999999994</v>
+      </c>
+      <c r="L77" s="3">
+        <v>0.37</v>
+      </c>
+      <c r="M77" s="3">
+        <v>14.1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B78" s="1">
+        <v>22</v>
+      </c>
+      <c r="C78" s="3">
+        <v>91.5</v>
+      </c>
+      <c r="D78" s="3">
+        <v>51.6</v>
+      </c>
+      <c r="E78" s="3">
+        <v>3</v>
+      </c>
+      <c r="F78" s="3">
+        <v>74.900000000000006</v>
+      </c>
+      <c r="G78" s="3">
+        <v>1.68</v>
+      </c>
+      <c r="H78" s="3">
+        <v>5.74</v>
+      </c>
+      <c r="I78" s="3">
+        <v>2.57</v>
+      </c>
+      <c r="J78" s="3">
+        <v>2</v>
+      </c>
+      <c r="K78" s="3">
+        <v>82.8</v>
+      </c>
+      <c r="L78" s="3">
+        <v>0.47</v>
+      </c>
+      <c r="M78" s="3">
+        <v>14.6</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B79" s="1">
+        <v>22</v>
+      </c>
+      <c r="C79" s="3">
+        <v>86.5</v>
+      </c>
+      <c r="D79" s="3">
+        <v>50.8</v>
+      </c>
+      <c r="E79" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F79" s="3">
+        <v>73.3</v>
+      </c>
+      <c r="G79" s="3">
+        <v>2.29</v>
+      </c>
+      <c r="H79" s="3">
+        <v>5.05</v>
+      </c>
+      <c r="I79" s="3">
+        <v>5.17</v>
+      </c>
+      <c r="J79" s="3">
+        <v>1.49</v>
+      </c>
+      <c r="K79" s="3">
+        <v>71.7</v>
+      </c>
+      <c r="L79" s="3">
+        <v>0.36</v>
+      </c>
+      <c r="M79" s="3">
+        <v>13.4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B80" s="1">
+        <v>22</v>
+      </c>
+      <c r="C80" s="3">
+        <v>87</v>
+      </c>
+      <c r="D80" s="3">
+        <v>56.7</v>
+      </c>
+      <c r="E80" s="3">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="F80" s="3">
+        <v>75.099999999999994</v>
+      </c>
+      <c r="G80" s="3">
+        <v>2.71</v>
+      </c>
+      <c r="H80" s="3">
+        <v>6.11</v>
+      </c>
+      <c r="I80" s="3">
+        <v>4.12</v>
+      </c>
+      <c r="J80" s="3">
+        <v>2.6</v>
+      </c>
+      <c r="K80" s="3">
+        <v>89.1</v>
+      </c>
+      <c r="L80" s="3">
+        <v>0.46</v>
+      </c>
+      <c r="M80" s="3">
+        <v>18.899999999999999</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B81" s="1">
+        <v>26</v>
+      </c>
+      <c r="C81" s="3">
+        <v>59</v>
+      </c>
+      <c r="D81" s="3">
+        <v>56.1</v>
+      </c>
+      <c r="E81" s="3">
+        <v>3.3</v>
+      </c>
+      <c r="F81" s="3">
+        <v>70.2</v>
+      </c>
+      <c r="G81" s="3">
+        <v>2.31</v>
+      </c>
+      <c r="H81" s="3">
+        <v>6.57</v>
+      </c>
+      <c r="I81" s="3">
+        <v>3.06</v>
+      </c>
+      <c r="J81" s="3">
+        <v>2.02</v>
+      </c>
+      <c r="K81" s="3">
+        <v>78.8</v>
+      </c>
+      <c r="L81" s="3">
+        <v>0.36</v>
+      </c>
+      <c r="M81" s="3">
+        <v>16.7</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B82" s="1">
+        <v>26</v>
+      </c>
+      <c r="C82" s="3">
+        <v>60.5</v>
+      </c>
+      <c r="D82" s="3">
+        <v>53.8</v>
+      </c>
+      <c r="E82" s="3">
+        <v>3.8</v>
+      </c>
+      <c r="F82" s="3">
+        <v>68</v>
+      </c>
+      <c r="G82" s="3">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="H82" s="3">
+        <v>7.1</v>
+      </c>
+      <c r="I82" s="3">
+        <v>5.0199999999999996</v>
+      </c>
+      <c r="J82" s="3">
+        <v>1.71</v>
+      </c>
+      <c r="K82" s="3">
+        <v>92.3</v>
+      </c>
+      <c r="L82" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="M82" s="3">
+        <v>21.2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B83" s="1">
+        <v>26</v>
+      </c>
+      <c r="C83" s="3">
+        <v>65.5</v>
+      </c>
+      <c r="D83" s="3">
+        <v>54.3</v>
+      </c>
+      <c r="E83" s="3">
+        <v>3.8</v>
+      </c>
+      <c r="F83" s="3">
+        <v>69.8</v>
+      </c>
+      <c r="G83" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="H83" s="3">
+        <v>7.84</v>
+      </c>
+      <c r="I83" s="3">
+        <v>5.52</v>
+      </c>
+      <c r="J83" s="3">
+        <v>1.7</v>
+      </c>
+      <c r="K83" s="3">
+        <v>84.4</v>
+      </c>
+      <c r="L83" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="M83" s="3">
+        <v>16.899999999999999</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B84" s="1">
+        <v>26</v>
+      </c>
+      <c r="C84" s="3">
+        <v>70</v>
+      </c>
+      <c r="D84" s="3">
+        <v>53.7</v>
+      </c>
+      <c r="E84" s="3">
+        <v>2.6</v>
+      </c>
+      <c r="F84" s="3">
+        <v>69.8</v>
+      </c>
+      <c r="G84" s="3">
+        <v>1.8</v>
+      </c>
+      <c r="H84" s="3">
+        <v>6.14</v>
+      </c>
+      <c r="I84" s="3">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="J84" s="3">
+        <v>1.75</v>
+      </c>
+      <c r="K84" s="3">
+        <v>68.5</v>
+      </c>
+      <c r="L84" s="3">
+        <v>0.43</v>
+      </c>
+      <c r="M84" s="3">
+        <v>19.2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A85" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B85" s="1">
         <v>30</v>
       </c>
-      <c r="C74" s="3">
+      <c r="C85" s="3">
         <v>66</v>
       </c>
-      <c r="D74" s="5">
+      <c r="D85" s="5">
         <v>53.1</v>
       </c>
-      <c r="E74" s="5">
+      <c r="E85" s="5">
         <v>1.52</v>
       </c>
-      <c r="F74" s="5">
+      <c r="F85" s="5">
         <v>69.7</v>
       </c>
-      <c r="G74" s="5">
+      <c r="G85" s="5">
         <v>1.03</v>
       </c>
-      <c r="H74" s="5">
+      <c r="H85" s="5">
         <v>5.21</v>
       </c>
-      <c r="I74" s="5">
+      <c r="I85" s="5">
         <v>4.18</v>
       </c>
-      <c r="J74" s="5">
+      <c r="J85" s="5">
         <v>0.17</v>
       </c>
-      <c r="K74" s="3">
+      <c r="K85" s="3">
         <v>43.1</v>
       </c>
-      <c r="L74" s="3">
+      <c r="L85" s="3">
         <v>0.33</v>
       </c>
-      <c r="M74" s="8">
+      <c r="M85" s="8">
         <v>11.4</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A75" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B75" s="1">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A86" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B86" s="1">
         <v>30</v>
       </c>
-      <c r="C75" s="3">
+      <c r="C86" s="3">
         <v>93</v>
       </c>
-      <c r="D75" s="5">
+      <c r="D86" s="5">
         <v>49.2</v>
       </c>
-      <c r="E75" s="5">
+      <c r="E86" s="5">
         <v>1.84</v>
       </c>
-      <c r="F75" s="5">
+      <c r="F86" s="5">
         <v>76.5</v>
       </c>
-      <c r="G75" s="5">
+      <c r="G86" s="5">
         <v>1.28</v>
       </c>
-      <c r="H75" s="5">
+      <c r="H86" s="5">
         <v>5.04</v>
       </c>
-      <c r="I75" s="5">
+      <c r="I86" s="5">
         <v>3.78</v>
       </c>
-      <c r="J75" s="5">
+      <c r="J86" s="5">
         <v>0.51</v>
       </c>
-      <c r="K75" s="3">
+      <c r="K86" s="3">
         <v>65.8</v>
       </c>
-      <c r="L75" s="3">
+      <c r="L86" s="3">
         <v>0.32</v>
       </c>
-      <c r="M75" s="3">
+      <c r="M86" s="3">
         <v>17.600000000000001</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A76" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B76" s="1">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A87" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B87" s="1">
         <v>30</v>
       </c>
-      <c r="C76" s="3">
+      <c r="C87" s="3">
         <v>119</v>
       </c>
-      <c r="D76" s="3">
+      <c r="D87" s="3">
         <v>44.1</v>
       </c>
-      <c r="E76" s="3">
-        <v>2</v>
-      </c>
-      <c r="F76" s="3">
+      <c r="E87" s="3">
+        <v>2</v>
+      </c>
+      <c r="F87" s="3">
         <v>77.900000000000006</v>
       </c>
-      <c r="G76" s="3">
+      <c r="G87" s="3">
         <v>1.26</v>
       </c>
-      <c r="H76" s="3">
+      <c r="H87" s="3">
         <v>4.76</v>
       </c>
-      <c r="I76" s="3">
+      <c r="I87" s="3">
         <v>2.8</v>
       </c>
-      <c r="J76" s="5">
+      <c r="J87" s="5">
         <v>0.73</v>
       </c>
-      <c r="K76" s="3">
+      <c r="K87" s="3">
         <v>58.9</v>
       </c>
-      <c r="L76" s="3">
+      <c r="L87" s="3">
         <v>0.4</v>
       </c>
-      <c r="M76" s="3">
+      <c r="M87" s="3">
         <v>22.5</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A77" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B77" s="1">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A88" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B88" s="1">
         <v>30</v>
       </c>
-      <c r="C77" s="3">
+      <c r="C88" s="3">
         <v>97</v>
       </c>
-      <c r="D77" s="4">
+      <c r="D88" s="4">
         <v>44.6</v>
       </c>
-      <c r="E77" s="4">
+      <c r="E88" s="4">
         <v>1.97</v>
       </c>
-      <c r="F77" s="4">
+      <c r="F88" s="4">
         <v>82.7</v>
       </c>
-      <c r="G77" s="4">
+      <c r="G88" s="4">
         <v>1.28</v>
       </c>
-      <c r="H77" s="3">
+      <c r="H88" s="3">
         <v>4.33</v>
       </c>
-      <c r="I77" s="3">
+      <c r="I88" s="3">
         <v>2.92</v>
       </c>
-      <c r="J77" s="3">
+      <c r="J88" s="3">
         <v>0.54</v>
       </c>
-      <c r="K77" s="3">
+      <c r="K88" s="3">
         <v>67.7</v>
       </c>
-      <c r="L77" s="3">
+      <c r="L88" s="3">
         <v>0.42</v>
       </c>
-      <c r="M77" s="3">
+      <c r="M88" s="3">
         <v>31.2</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A78" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B78" s="1">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A89" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B89" s="1">
         <v>30</v>
       </c>
-      <c r="C78" s="3">
+      <c r="C89" s="3">
         <v>90</v>
       </c>
-      <c r="D78" s="4">
+      <c r="D89" s="4">
         <v>44.9</v>
       </c>
-      <c r="E78" s="4">
+      <c r="E89" s="4">
         <v>1.81</v>
       </c>
-      <c r="F78" s="4">
+      <c r="F89" s="4">
         <v>81.5</v>
       </c>
-      <c r="G78" s="4">
+      <c r="G89" s="4">
         <v>1.24</v>
       </c>
-      <c r="H78" s="3">
+      <c r="H89" s="3">
         <v>5.6</v>
       </c>
-      <c r="I78" s="3">
+      <c r="I89" s="3">
         <v>2.9</v>
       </c>
-      <c r="J78" s="3">
+      <c r="J89" s="3">
         <v>0.71</v>
       </c>
-      <c r="K78" s="3">
+      <c r="K89" s="3">
         <v>64</v>
       </c>
-      <c r="L78" s="3">
+      <c r="L89" s="3">
         <v>0.35</v>
       </c>
-      <c r="M78" s="3">
+      <c r="M89" s="3">
         <v>18.2</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A79" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B79" s="1">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A90" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B90" s="1">
         <v>30</v>
       </c>
-      <c r="C79" s="3">
+      <c r="C90" s="3">
         <v>131.6</v>
       </c>
-      <c r="D79" s="3">
+      <c r="D90" s="3">
         <v>46.5</v>
       </c>
-      <c r="E79" s="3">
+      <c r="E90" s="3">
         <v>2.91</v>
       </c>
-      <c r="F79" s="3">
+      <c r="F90" s="3">
         <v>82.2</v>
       </c>
-      <c r="G79" s="3">
+      <c r="G90" s="3">
         <v>1.7</v>
       </c>
-      <c r="H79" s="3">
+      <c r="H90" s="3">
         <v>2.35</v>
       </c>
-      <c r="I79" s="3">
+      <c r="I90" s="3">
         <v>4.0599999999999996</v>
       </c>
-      <c r="J79" s="3">
+      <c r="J90" s="3">
         <v>1.21</v>
       </c>
-      <c r="K79" s="3">
+      <c r="K90" s="3">
         <v>94</v>
       </c>
-      <c r="L79" s="3">
+      <c r="L90" s="3">
         <v>0.19</v>
       </c>
-      <c r="M79" s="3">
+      <c r="M90" s="3">
         <v>7.9</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A80" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B80" s="1">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A91" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B91" s="1">
         <v>30</v>
       </c>
-      <c r="C80" s="3">
+      <c r="C91" s="3">
         <v>74.2</v>
       </c>
-      <c r="D80" s="3">
+      <c r="D91" s="3">
         <v>41.5</v>
       </c>
-      <c r="E80" s="3">
+      <c r="E91" s="3">
         <v>2.02</v>
       </c>
-      <c r="F80" s="3">
+      <c r="F91" s="3">
         <v>87.7</v>
       </c>
-      <c r="G80" s="3">
+      <c r="G91" s="3">
         <v>1.24</v>
       </c>
-      <c r="H80" s="3">
+      <c r="H91" s="3">
         <v>2.09</v>
       </c>
-      <c r="I80" s="3">
+      <c r="I91" s="3">
         <v>4.79</v>
       </c>
-      <c r="J80" s="3">
+      <c r="J91" s="3">
         <v>0.84</v>
       </c>
-      <c r="K80" s="3">
+      <c r="K91" s="3">
         <v>68</v>
       </c>
-      <c r="L80" s="3">
+      <c r="L91" s="3">
         <v>0.24</v>
       </c>
-      <c r="M80" s="3">
+      <c r="M91" s="3">
         <v>12.2</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A81" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B81" s="1">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A92" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B92" s="1">
         <v>30</v>
       </c>
-      <c r="C81" s="3">
+      <c r="C92" s="3">
         <v>69.8</v>
       </c>
-      <c r="D81" s="3">
+      <c r="D92" s="3">
         <v>47.9</v>
       </c>
-      <c r="E81" s="3">
+      <c r="E92" s="3">
         <v>1.55</v>
       </c>
-      <c r="F81" s="3">
+      <c r="F92" s="3">
         <v>82.3</v>
       </c>
-      <c r="G81" s="3">
+      <c r="G92" s="3">
         <v>0.86</v>
       </c>
-      <c r="H81" s="3">
+      <c r="H92" s="3">
         <v>2.2400000000000002</v>
       </c>
-      <c r="I81" s="3">
+      <c r="I92" s="3">
         <v>4.6900000000000004</v>
       </c>
-      <c r="J81" s="3">
+      <c r="J92" s="3">
         <v>0.28000000000000003</v>
       </c>
-      <c r="K81" s="3">
+      <c r="K92" s="3">
         <v>77.2</v>
       </c>
-      <c r="L81" s="3">
+      <c r="L92" s="3">
         <v>0.21</v>
       </c>
-      <c r="M81" s="3">
+      <c r="M92" s="3">
         <v>12.5</v>
       </c>
     </row>

</xml_diff>